<commit_message>
Reordenacion de pruebas + inicio de excel
</commit_message>
<xml_diff>
--- a/tecnicaCajaNegra.xlsx
+++ b/tecnicaCajaNegra.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carolam\Desktop\UNI\2º-CUATRI\INGENIERIA DEL SOFTWARE 2\IS2_2122\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Moodle\Tercer Curso\SegundoCuatrimestre\IngenieriaSoftwareII\IS2_2122\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEF636B-1736-424A-A1F8-5A5B277B4CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5950D7B5-4A55-4962-B1B3-72CE8ED1CA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B7E8EB2-CB6A-44E4-9B29-750F352AD572}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8B7E8EB2-CB6A-44E4-9B29-750F352AD572}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="CajaNegra" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>TURISMO</t>
   </si>
@@ -83,13 +84,133 @@
   </si>
   <si>
     <t>motocicleta(cilindrada)</t>
+  </si>
+  <si>
+    <t>Turismo</t>
+  </si>
+  <si>
+    <t>Clase Turismo</t>
+  </si>
+  <si>
+    <t>Clases Validas</t>
+  </si>
+  <si>
+    <t>Clases No validas</t>
+  </si>
+  <si>
+    <t>Matrícula</t>
+  </si>
+  <si>
+    <t>FechaMatriculacion</t>
+  </si>
+  <si>
+    <t>Potencia</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>!string, null</t>
+  </si>
+  <si>
+    <t>!fecha, null</t>
+  </si>
+  <si>
+    <t>fecha (localDate)</t>
+  </si>
+  <si>
+    <t>double, &gt;0</t>
+  </si>
+  <si>
+    <t>!double, &lt;=0 null</t>
+  </si>
+  <si>
+    <t>Casos de Prueba</t>
+  </si>
+  <si>
+    <t>ValorEsperado</t>
+  </si>
+  <si>
+    <t>("12569PO", LocalDate.now().minusYears(26), 12.85):</t>
+  </si>
+  <si>
+    <t>("23954KOP", LocalDate.now().plusDays(5), 74.23):</t>
+  </si>
+  <si>
+    <t>("52369ACF", LocalDate.now(), 19.85):</t>
+  </si>
+  <si>
+    <t>("552FRFRE", LocalDate.now().minusDays(41), 16.41):</t>
+  </si>
+  <si>
+    <t>("65456ADEF", LocalDate.now().minusDays(39), 15.98):</t>
+  </si>
+  <si>
+    <t>("569931", LocalDate.now().plusDays(14), 12.03):</t>
+  </si>
+  <si>
+    <t>("542DDS", LocalDate.now().plusDays(10), 11.95):</t>
+  </si>
+  <si>
+    <t>("ABBA1235", LocalDate.now().minusDays(1), 8.50):</t>
+  </si>
+  <si>
+    <t>("1321", LocalDate.now().plusDays(4), 7.90):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now().plusDays(1), 1):</t>
+  </si>
+  <si>
+    <t>("51385LK", LocalDate.now().minusYears(25), 114):</t>
+  </si>
+  <si>
+    <t>PrecioImpuesto</t>
+  </si>
+  <si>
+    <t>Clase Furgoneta</t>
+  </si>
+  <si>
+    <t>Valores</t>
+  </si>
+  <si>
+    <t>Columna4</t>
+  </si>
+  <si>
+    <t>1. 1234</t>
+  </si>
+  <si>
+    <t>2. hoy</t>
+  </si>
+  <si>
+    <t>3. 21</t>
+  </si>
+  <si>
+    <t>4. 12</t>
+  </si>
+  <si>
+    <t>5. null</t>
+  </si>
+  <si>
+    <t>6. 25</t>
+  </si>
+  <si>
+    <t>7.null</t>
+  </si>
+  <si>
+    <t>8. "hola"</t>
+  </si>
+  <si>
+    <t>9. -0.99</t>
+  </si>
+  <si>
+    <t>10. null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,16 +218,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -114,11 +260,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -126,11 +367,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -141,6 +417,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{010405D1-FAAC-4404-94C9-F10767BF9EBA}" name="Tabla2" displayName="Tabla2" ref="G4:H15" totalsRowShown="0">
+  <autoFilter ref="G4:H15" xr:uid="{010405D1-FAAC-4404-94C9-F10767BF9EBA}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{EBA2B40D-7824-4711-AC26-09AAE2E789F1}" name="Casos de Prueba" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{8C7346ED-F76B-4CF5-BA59-AAA305746A9E}" name="ValorEsperado" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,28 +726,237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275440AC-4520-4206-A9FA-8D187B524CA7}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="4">
+        <v>25.24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="4">
+        <v>25.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="4">
+        <v>68.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="4">
+        <v>68.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="4">
+        <v>143.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="4">
+        <v>143.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="4">
+        <v>179.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="4">
+        <v>179.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="G15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EB088C-FC0A-4755-A918-62E77BA3612A}">
   <dimension ref="B4:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -489,7 +985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -518,7 +1014,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -529,7 +1025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -540,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L8" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Tecnicas de Caja Negra Teórica
</commit_message>
<xml_diff>
--- a/tecnicaCajaNegra.xlsx
+++ b/tecnicaCajaNegra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Moodle\Tercer Curso\SegundoCuatrimestre\IngenieriaSoftwareII\IS2_2122\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6D1A83-EF7B-4395-A483-64C7637248B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A970512-0A6D-4F65-91D4-8600E25B76BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8B7E8EB2-CB6A-44E4-9B29-750F352AD572}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="129">
   <si>
     <t>TURISMO</t>
   </si>
@@ -107,24 +107,6 @@
     <t>Potencia</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>!string, null</t>
-  </si>
-  <si>
-    <t>!fecha, null</t>
-  </si>
-  <si>
-    <t>fecha (localDate)</t>
-  </si>
-  <si>
-    <t>double, &gt;0</t>
-  </si>
-  <si>
-    <t>!double, &lt;=0 null</t>
-  </si>
-  <si>
     <t>Casos de Prueba</t>
   </si>
   <si>
@@ -164,84 +146,33 @@
     <t>("51385LK", LocalDate.now().minusYears(25), 114):</t>
   </si>
   <si>
-    <t>PrecioImpuesto</t>
-  </si>
-  <si>
     <t>Clase Furgoneta</t>
   </si>
   <si>
     <t>Valores</t>
   </si>
   <si>
-    <t>1. 1234</t>
-  </si>
-  <si>
     <t>2. hoy</t>
   </si>
   <si>
     <t>3. 21</t>
   </si>
   <si>
-    <t>4. 12</t>
-  </si>
-  <si>
-    <t>5. null</t>
-  </si>
-  <si>
-    <t>6. 25</t>
-  </si>
-  <si>
-    <t>7.null</t>
-  </si>
-  <si>
-    <t>8. "hola"</t>
-  </si>
-  <si>
-    <t>9. -0.99</t>
-  </si>
-  <si>
-    <t>10. null</t>
-  </si>
-  <si>
     <t>Furgoneta</t>
   </si>
   <si>
     <t>Comercial</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>!boolean, null</t>
-  </si>
-  <si>
     <t>4. True</t>
   </si>
   <si>
-    <t>12. null</t>
-  </si>
-  <si>
     <t>5. 2345</t>
   </si>
   <si>
-    <t>6. hoy +2 dias</t>
-  </si>
-  <si>
     <t>7. 50</t>
   </si>
   <si>
-    <t>8.false</t>
-  </si>
-  <si>
-    <t>9. 5616</t>
-  </si>
-  <si>
-    <t>10.hace 20 dias</t>
-  </si>
-  <si>
-    <t>11. -0.99</t>
-  </si>
-  <si>
     <t>("1234", LocalDate.now().plusDays(1), 1, false):</t>
   </si>
   <si>
@@ -276,13 +207,229 @@
   </si>
   <si>
     <t>("51385LK", LocalDate.now().minusYears(25), 65.32, true):</t>
+  </si>
+  <si>
+    <t>String(1)</t>
+  </si>
+  <si>
+    <t>fecha (localDate)(2)</t>
+  </si>
+  <si>
+    <t>!string(5), null(6)</t>
+  </si>
+  <si>
+    <t>!fecha(7), null(8)</t>
+  </si>
+  <si>
+    <t>!double(9), &lt;=0(10) null(11)</t>
+  </si>
+  <si>
+    <t>1. "1234"</t>
+  </si>
+  <si>
+    <t>4. 12.5</t>
+  </si>
+  <si>
+    <t>9. "hola"</t>
+  </si>
+  <si>
+    <t>11. null</t>
+  </si>
+  <si>
+    <t>5. 45</t>
+  </si>
+  <si>
+    <t>6. null</t>
+  </si>
+  <si>
+    <t>7. 99</t>
+  </si>
+  <si>
+    <t>8 null</t>
+  </si>
+  <si>
+    <t>Casos De prueba</t>
+  </si>
+  <si>
+    <t>Turismo("1234", 12, 21)</t>
+  </si>
+  <si>
+    <t>Turismo("2345", null, 12.5)</t>
+  </si>
+  <si>
+    <t>Turismo(45, mañana, 12.5)</t>
+  </si>
+  <si>
+    <t>Turismo("1234", hoy, "hola")</t>
+  </si>
+  <si>
+    <t>Turismo("1234", hoy, null)</t>
+  </si>
+  <si>
+    <t>10. -1</t>
+  </si>
+  <si>
+    <t>Turismo("1234", hoy, 40)</t>
+  </si>
+  <si>
+    <t>Turismo("5616", hoy, -1)</t>
+  </si>
+  <si>
+    <t>3. 40</t>
+  </si>
+  <si>
+    <t>Turismo(null, ayer, 1)</t>
+  </si>
+  <si>
+    <t>double &gt;0 (3)</t>
+  </si>
+  <si>
+    <t>boolean(4)</t>
+  </si>
+  <si>
+    <t>8. null</t>
+  </si>
+  <si>
+    <t>!boolean(12), null(13)</t>
+  </si>
+  <si>
+    <t>13. null</t>
+  </si>
+  <si>
+    <t>12. 2</t>
+  </si>
+  <si>
+    <t>10.-0.99</t>
+  </si>
+  <si>
+    <t>Furgoneta("1234", hoy, 21, true)</t>
+  </si>
+  <si>
+    <t>Furgoneta(2345, hace 20 dias, 1, true)</t>
+  </si>
+  <si>
+    <t>Furgoneta(null, hace 20 dias, 1, true)</t>
+  </si>
+  <si>
+    <t>Furgoneta("4684", 50, 12.5, false)</t>
+  </si>
+  <si>
+    <t>Furgoneta("4684", null, 12.5, false)</t>
+  </si>
+  <si>
+    <t>Furgoneta("5616", hoy, -0.99, true)</t>
+  </si>
+  <si>
+    <t>Furgoneta("5616", hoy, "hola", true)</t>
+  </si>
+  <si>
+    <t>Furgoneta("5616", hoy,null, true)</t>
+  </si>
+  <si>
+    <t>Furgoneta("5616", hoy, "hola, null)</t>
+  </si>
+  <si>
+    <t>Id valores</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>id valores</t>
+  </si>
+  <si>
+    <t>double &gt;0(3)</t>
+  </si>
+  <si>
+    <t>!string(4), null(5)</t>
+  </si>
+  <si>
+    <t>!fecha(6), null(7)</t>
+  </si>
+  <si>
+    <t>!double(8), &lt;=0(9) null(10)</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>PrecioImpuesto()</t>
+  </si>
+  <si>
+    <t>precioImpuesto()</t>
+  </si>
+  <si>
+    <t>Clase Motocicleta</t>
+  </si>
+  <si>
+    <t>Motocicleta</t>
+  </si>
+  <si>
+    <t>3. 49</t>
+  </si>
+  <si>
+    <t>Motocicleta("1234", hoy, 40)</t>
+  </si>
+  <si>
+    <t>Motocicleta(45, mañana, 12.5)</t>
+  </si>
+  <si>
+    <t>Motocicleta(null, ayer, 1)</t>
+  </si>
+  <si>
+    <t>Motocicleta("1234", 12, 21)</t>
+  </si>
+  <si>
+    <t>Motocicleta("1234", hoy, "hola")</t>
+  </si>
+  <si>
+    <t>Motocicleta("1234", hoy, null)</t>
+  </si>
+  <si>
+    <t>Motocicleta("1234", null, 51)</t>
+  </si>
+  <si>
+    <t>Motocicleta("1234", hoy, -50)</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now(), 1):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now(), 50):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now(), 125):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now(), 249):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now(), 250):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now(), 499):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now(), 500):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now(), 999):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now(), 1000):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now().minusYears(25), 1748):</t>
+  </si>
+  <si>
+    <t>("1234", LocalDate.now()minusYears(26), 500):</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +444,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +501,26 @@
         <bgColor theme="4" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor theme="4" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -427,11 +623,120 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -450,8 +755,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -460,18 +763,61 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -498,22 +844,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{010405D1-FAAC-4404-94C9-F10767BF9EBA}" name="Tabla2" displayName="Tabla2" ref="G4:H15" totalsRowShown="0">
-  <autoFilter ref="G4:H15" xr:uid="{010405D1-FAAC-4404-94C9-F10767BF9EBA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{010405D1-FAAC-4404-94C9-F10767BF9EBA}" name="Tabla2" displayName="Tabla2" ref="L4:M15" totalsRowShown="0">
+  <autoFilter ref="L4:M15" xr:uid="{010405D1-FAAC-4404-94C9-F10767BF9EBA}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EBA2B40D-7824-4711-AC26-09AAE2E789F1}" name="Casos de Prueba" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{8C7346ED-F76B-4CF5-BA59-AAA305746A9E}" name="ValorEsperado" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{EBA2B40D-7824-4711-AC26-09AAE2E789F1}" name="Casos de Prueba" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8C7346ED-F76B-4CF5-BA59-AAA305746A9E}" name="ValorEsperado" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF9C19B6-BC36-4490-8F0F-F26905FF15B4}" name="Tabla22" displayName="Tabla22" ref="G24:H36" totalsRowShown="0">
-  <autoFilter ref="G24:H36" xr:uid="{EF9C19B6-BC36-4490-8F0F-F26905FF15B4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF9C19B6-BC36-4490-8F0F-F26905FF15B4}" name="Tabla22" displayName="Tabla22" ref="L27:M39" totalsRowShown="0">
+  <autoFilter ref="L27:M39" xr:uid="{EF9C19B6-BC36-4490-8F0F-F26905FF15B4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6E82589E-C63F-4924-955F-D0E664A60B7B}" name="Casos de Prueba" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{02EF6B4E-8FA0-4E1C-981C-E745CCB96025}" name="ValorEsperado" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6E82589E-C63F-4924-955F-D0E664A60B7B}" name="Casos de Prueba" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{02EF6B4E-8FA0-4E1C-981C-E745CCB96025}" name="ValorEsperado" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E54209B0-68A6-464C-BE3E-670C4EE59A28}" name="Tabla24" displayName="Tabla24" ref="L49:M60" totalsRowShown="0">
+  <autoFilter ref="L49:M60" xr:uid="{E54209B0-68A6-464C-BE3E-670C4EE59A28}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D918EA40-880F-4EF6-BC88-2623B914B94D}" name="Casos de Prueba" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{9CFA7683-A0A0-4800-B0FC-D74FD4FF190E}" name="ValorEsperado" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -816,405 +1173,790 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275440AC-4520-4206-A9FA-8D187B524CA7}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="53" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="53.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="31">
+        <v>4</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="4">
+        <v>25.24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="23">
+        <v>5</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="4">
+        <v>25.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="31">
+        <v>6</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="4">
+        <v>68.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F8" s="23">
+        <v>7</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="4">
+        <v>68.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F9" s="31">
+        <v>8</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="4">
+        <v>143.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="23">
+        <v>9</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="M10" s="4">
+        <v>143.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="31">
+        <v>10</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="4">
+        <v>179.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="4">
+        <v>179.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="L15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" s="4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="B28" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M28" s="4">
         <v>25.24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="4">
-        <v>25.24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="4">
-        <v>68.16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="4">
-        <v>68.16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="4">
-        <v>143.88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="4">
-        <v>143.88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="4">
-        <v>179.22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="4">
-        <v>179.22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="B29" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="23">
+        <v>5</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="L29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="4">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="G15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="4">
-        <v>25.24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H26" s="4">
+      <c r="M29" s="4">
         <f>25.24*0.8</f>
         <v>20.192</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H27" s="4">
+      <c r="B30" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="31">
+        <v>6</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M30" s="4">
         <f>68.16*0.8</f>
         <v>54.527999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H28" s="4">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="23">
+        <v>7</v>
+      </c>
+      <c r="G31" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M31" s="4">
         <v>68.16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" s="4">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F32" s="31">
+        <v>8</v>
+      </c>
+      <c r="G32" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M32" s="4">
         <v>143.88</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H30" s="4">
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="23">
+        <v>9</v>
+      </c>
+      <c r="G33" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" s="4">
         <f>143.88*0.8</f>
         <v>115.104</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H31" s="4">
+    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="F34" s="31">
+        <v>10</v>
+      </c>
+      <c r="G34" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M34" s="4">
         <f>179.22*0.8</f>
         <v>143.376</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H32" s="4">
+    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="23">
+        <v>11</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M35" s="4">
         <v>179.22</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H33" s="4">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="F36" s="31">
+        <v>12</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M36" s="4">
         <f>224*0.8</f>
         <v>179.20000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H34" s="4">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="25"/>
+      <c r="F37" s="23">
+        <v>13</v>
+      </c>
+      <c r="G37" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M37" s="4">
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H35" s="4">
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="25"/>
+      <c r="L38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M38" s="4">
         <f>224*0.8</f>
         <v>179.20000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G36" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H36" s="4">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G47" s="30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F48" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="L48" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="G49" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F50" s="31">
+        <v>4</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L50" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="M50" s="4">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51" s="23">
+        <v>5</v>
+      </c>
+      <c r="G51" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="L51" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="M51" s="4">
+        <v>25.24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F52" s="31">
+        <v>6</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="L52" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="M52" s="4">
+        <v>68.16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F53" s="23">
+        <v>7</v>
+      </c>
+      <c r="G53" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="L53" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="M53" s="4">
+        <v>68.16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F54" s="31">
+        <v>8</v>
+      </c>
+      <c r="G54" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="L54" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="M54" s="4">
+        <v>143.88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F55" s="23">
+        <v>9</v>
+      </c>
+      <c r="G55" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="L55" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="M55" s="4">
+        <v>143.88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="31">
+        <v>10</v>
+      </c>
+      <c r="G56" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="L56" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="M56" s="4">
+        <v>179.22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L57" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="M57" s="4">
+        <v>179.22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="L58" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M58" s="4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L59" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="M59" s="4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="15"/>
+      <c r="L60" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="M60" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Falta arreglar add y remove
</commit_message>
<xml_diff>
--- a/tecnicaCajaNegra.xlsx
+++ b/tecnicaCajaNegra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Moodle\Tercer Curso\SegundoCuatrimestre\IngenieriaSoftwareII\IS2_2122\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carolam\Desktop\UNI\2º-CUATRI\INGENIERIA DEL SOFTWARE 2\IS2_2122\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2273D3-B945-487D-9F0A-4C067A3BE2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6DA196-61A6-4D7A-BD16-CC21A8DF6AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8B7E8EB2-CB6A-44E4-9B29-750F352AD572}"/>
+    <workbookView xWindow="10452" yWindow="3120" windowWidth="10140" windowHeight="8016" activeTab="1" xr2:uid="{8B7E8EB2-CB6A-44E4-9B29-750F352AD572}"/>
   </bookViews>
   <sheets>
     <sheet name="CajaNegra" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="200">
   <si>
     <t>Turismo</t>
   </si>
@@ -539,21 +538,6 @@
     <t>remove(1)</t>
   </si>
   <si>
-    <t>remove(2)</t>
-  </si>
-  <si>
-    <t>:8, [4,7]</t>
-  </si>
-  <si>
-    <t>(2,[4,7,8])</t>
-  </si>
-  <si>
-    <t>(1,[4,7])</t>
-  </si>
-  <si>
-    <t>:7, [4]</t>
-  </si>
-  <si>
     <t>(0,[4])</t>
   </si>
   <si>
@@ -644,17 +628,29 @@
     <t>remove(-3)</t>
   </si>
   <si>
-    <t>(-7, [1,5,6,9])</t>
-  </si>
-  <si>
     <t>En el método add habria que comprobar tambien que se añade adecuadamente.</t>
+  </si>
+  <si>
+    <t>(1,[4,7,8])</t>
+  </si>
+  <si>
+    <t>:7, [4,8]</t>
+  </si>
+  <si>
+    <t>:8, [4]</t>
+  </si>
+  <si>
+    <t>(1,[4,8])</t>
+  </si>
+  <si>
+    <t>(-3, [1,5,6,9])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1226,68 +1222,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1302,33 +1259,72 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1732,30 +1728,30 @@
       <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="53.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="53.88671875" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.6">
       <c r="G2" s="28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15" thickBot="1">
       <c r="F3" s="20" t="s">
         <v>83</v>
       </c>
@@ -1766,7 +1762,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
@@ -1789,7 +1785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="31" t="s">
         <v>4</v>
       </c>
@@ -1812,7 +1808,7 @@
         <v>25.24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
@@ -1835,7 +1831,7 @@
         <v>25.24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15" thickBot="1">
       <c r="A7" s="38" t="s">
         <v>6</v>
       </c>
@@ -1858,7 +1854,7 @@
         <v>68.16</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="F8" s="21">
         <v>7</v>
       </c>
@@ -1872,7 +1868,7 @@
         <v>68.16</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="F9" s="29">
         <v>8</v>
       </c>
@@ -1886,7 +1882,7 @@
         <v>143.88</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15" thickBot="1">
       <c r="F10" s="21">
         <v>9</v>
       </c>
@@ -1900,7 +1896,7 @@
         <v>143.88</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15" thickBot="1">
       <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
@@ -1917,7 +1913,7 @@
         <v>179.22</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="15" t="s">
         <v>46</v>
       </c>
@@ -1934,7 +1930,7 @@
         <v>179.22</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -1951,7 +1947,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1968,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>47</v>
       </c>
@@ -1983,12 +1979,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="16.2" thickBot="1">
       <c r="G26" s="28" t="s">
         <v>24</v>
       </c>
@@ -1996,7 +1992,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="15" thickBot="1">
       <c r="A27" s="30" t="s">
         <v>24</v>
       </c>
@@ -2019,7 +2015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="31" t="s">
         <v>4</v>
       </c>
@@ -2042,7 +2038,7 @@
         <v>25.24</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" s="32" t="s">
         <v>5</v>
       </c>
@@ -2066,7 +2062,7 @@
         <v>20.192</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" s="31" t="s">
         <v>6</v>
       </c>
@@ -2090,7 +2086,7 @@
         <v>54.527999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15" thickBot="1">
       <c r="A31" s="33" t="s">
         <v>25</v>
       </c>
@@ -2113,7 +2109,7 @@
         <v>68.16</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="F32" s="29">
         <v>8</v>
       </c>
@@ -2127,7 +2123,7 @@
         <v>143.88</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="15" thickBot="1">
       <c r="F33" s="21">
         <v>9</v>
       </c>
@@ -2142,7 +2138,7 @@
         <v>115.104</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="15" thickBot="1">
       <c r="A34" s="18" t="s">
         <v>21</v>
       </c>
@@ -2163,7 +2159,7 @@
         <v>143.376</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="15" thickBot="1">
       <c r="A35" s="4" t="s">
         <v>46</v>
       </c>
@@ -2189,7 +2185,7 @@
         <v>179.22</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" s="5" t="s">
         <v>22</v>
       </c>
@@ -2214,7 +2210,7 @@
         <v>179.20000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" s="4" t="s">
         <v>23</v>
       </c>
@@ -2238,7 +2234,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="15" thickBot="1">
       <c r="A38" s="12" t="s">
         <v>26</v>
       </c>
@@ -2257,7 +2253,7 @@
         <v>179.20000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="L39" s="1" t="s">
         <v>39</v>
       </c>
@@ -2265,17 +2261,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="15.6">
       <c r="G47" s="28" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="15" thickBot="1">
       <c r="F48" s="20" t="s">
         <v>83</v>
       </c>
@@ -2286,7 +2282,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" s="30" t="s">
         <v>92</v>
       </c>
@@ -2309,7 +2305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" s="31" t="s">
         <v>4</v>
       </c>
@@ -2332,7 +2328,7 @@
         <v>8.84</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" s="32" t="s">
         <v>5</v>
       </c>
@@ -2355,7 +2351,7 @@
         <v>25.24</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" ht="15" thickBot="1">
       <c r="A52" s="38" t="s">
         <v>6</v>
       </c>
@@ -2378,7 +2374,7 @@
         <v>68.16</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="F53" s="21">
         <v>7</v>
       </c>
@@ -2392,7 +2388,7 @@
         <v>68.16</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="F54" s="29">
         <v>8</v>
       </c>
@@ -2406,7 +2402,7 @@
         <v>143.88</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="15" thickBot="1">
       <c r="F55" s="21">
         <v>9</v>
       </c>
@@ -2420,7 +2416,7 @@
         <v>143.88</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="15" thickBot="1">
       <c r="A56" s="19" t="s">
         <v>21</v>
       </c>
@@ -2437,7 +2433,7 @@
         <v>179.22</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" s="15" t="s">
         <v>46</v>
       </c>
@@ -2454,7 +2450,7 @@
         <v>179.22</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" s="9" t="s">
         <v>22</v>
       </c>
@@ -2471,7 +2467,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" s="7" t="s">
         <v>93</v>
       </c>
@@ -2488,7 +2484,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" ht="15" thickBot="1">
       <c r="A60" s="11" t="s">
         <v>47</v>
       </c>
@@ -2518,28 +2514,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387CFE5F-C44C-4C88-9E0E-9757B7251501}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:9" ht="15.6">
+      <c r="A1" s="70" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="42"/>
-    </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="70"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1">
       <c r="A2" s="27" t="s">
         <v>114</v>
       </c>
@@ -2553,49 +2549,49 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="45.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="56" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="47.25" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="49" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="43.2">
       <c r="A5" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="56" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>121</v>
       </c>
@@ -2605,7 +2601,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>125</v>
       </c>
@@ -2615,355 +2611,355 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F9" s="43" t="s">
-        <v>200</v>
-      </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+    <row r="9" spans="1:9">
+      <c r="F9" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="B10" s="44"/>
+      <c r="B10" s="71"/>
       <c r="C10" t="s">
         <v>154</v>
       </c>
-      <c r="F10" s="55" t="s">
+      <c r="F10" s="88" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" s="88"/>
+      <c r="H10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1">
+      <c r="A11" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="77"/>
+      <c r="D11" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="77"/>
+      <c r="I11" s="42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="81" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="I12" s="51" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="73"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>140</v>
+      </c>
+      <c r="F13" s="73"/>
+      <c r="G13" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="I13" s="52" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="73"/>
+      <c r="B14" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="73"/>
+      <c r="G14" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="55"/>
-      <c r="H10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="57" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="G11" s="57" t="s">
-        <v>131</v>
-      </c>
-      <c r="H11" s="57"/>
-      <c r="I11" s="45" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="54" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="73" t="s">
-        <v>136</v>
-      </c>
-      <c r="F12" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="G12" s="54" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" s="54" t="s">
+      <c r="I14" s="52" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1">
+      <c r="A15" s="74"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" s="74"/>
+      <c r="G15" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="H15" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="I12" s="60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="46" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="74" t="s">
-        <v>140</v>
-      </c>
-      <c r="F13" s="61"/>
-      <c r="G13" s="46" t="s">
+      <c r="I15" s="53" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="75" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="F16" s="83" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>186</v>
+      </c>
+      <c r="I16" s="66" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1">
+      <c r="A17" s="78"/>
+      <c r="B17" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="64" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="84"/>
+      <c r="G17" s="55" t="s">
+        <v>187</v>
+      </c>
+      <c r="H17" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="I17" s="56" t="s">
         <v>188</v>
       </c>
-      <c r="H13" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="I13" s="62" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
-      <c r="B14" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>151</v>
-      </c>
-      <c r="D14" s="74" t="s">
-        <v>141</v>
-      </c>
-      <c r="F14" s="61"/>
-      <c r="G14" s="46" t="s">
-        <v>183</v>
-      </c>
-      <c r="H14" s="46" t="s">
-        <v>184</v>
-      </c>
-      <c r="I14" s="62" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="63"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" s="75" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="63"/>
-      <c r="G15" s="50" t="s">
-        <v>186</v>
-      </c>
-      <c r="H15" s="50" t="s">
-        <v>187</v>
-      </c>
-      <c r="I15" s="64" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" s="51" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="77" t="s">
-        <v>147</v>
-      </c>
-      <c r="F16" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="G16" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="H16" s="66" t="s">
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="78"/>
+      <c r="B18" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="64" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="85" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="H18" s="48" t="s">
+        <v>189</v>
+      </c>
+      <c r="I18" s="51" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1">
+      <c r="A19" s="76"/>
+      <c r="B19" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="F19" s="86"/>
+      <c r="G19" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="H19" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="I16" s="85" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="78"/>
-      <c r="B17" s="48" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="D17" s="79" t="s">
-        <v>153</v>
-      </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="68" t="s">
-        <v>192</v>
-      </c>
-      <c r="H17" s="52" t="s">
+      <c r="I19" s="52" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1">
+      <c r="A20" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="60" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" s="87"/>
+      <c r="G20" s="57" t="s">
+        <v>193</v>
+      </c>
+      <c r="H20" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="I20" s="53" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1">
+      <c r="A21" s="73"/>
+      <c r="B21" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="I17" s="69" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
-      <c r="B18" s="48" t="s">
-        <v>155</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="D18" s="79" t="s">
-        <v>157</v>
-      </c>
-      <c r="F18" s="82" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="54" t="s">
+      <c r="D21" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="67"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="63"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1">
+      <c r="A22" s="73"/>
+      <c r="B22" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="H18" s="54" t="s">
-        <v>194</v>
-      </c>
-      <c r="I18" s="60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="80"/>
-      <c r="B19" s="52" t="s">
-        <v>158</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>159</v>
-      </c>
-      <c r="D19" s="81" t="s">
-        <v>160</v>
-      </c>
-      <c r="F19" s="83"/>
-      <c r="G19" s="46" t="s">
+      <c r="C22" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="D22" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="H19" s="58" t="s">
-        <v>196</v>
-      </c>
-      <c r="I19" s="62" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="54" t="s">
+      <c r="F22" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="68"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="69"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1">
+      <c r="A23" s="74"/>
+      <c r="B23" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="C20" s="54" t="s">
-        <v>162</v>
-      </c>
-      <c r="D20" s="73" t="s">
-        <v>163</v>
-      </c>
-      <c r="F20" s="84"/>
-      <c r="G20" s="70" t="s">
-        <v>198</v>
-      </c>
-      <c r="H20" s="50" t="s">
-        <v>199</v>
-      </c>
-      <c r="I20" s="64" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="61"/>
-      <c r="B21" s="46" t="s">
+      <c r="C23" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="D23" s="62" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="D21" s="74" t="s">
-        <v>166</v>
-      </c>
-      <c r="F21" s="71" t="s">
-        <v>121</v>
-      </c>
-      <c r="G21" s="86"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="77"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61"/>
-      <c r="B22" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>168</v>
-      </c>
-      <c r="D22" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="F22" s="72" t="s">
+      <c r="C24" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1">
+      <c r="A25" s="76"/>
+      <c r="B25" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="87"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="88"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="63"/>
-      <c r="B23" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="C23" s="50" t="s">
-        <v>170</v>
-      </c>
-      <c r="D23" s="75" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="76" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" s="51" t="s">
-        <v>172</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>175</v>
-      </c>
-      <c r="D24" s="77" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
-      <c r="B25" s="52" t="s">
-        <v>172</v>
-      </c>
-      <c r="C25" s="52" t="s">
+      <c r="B26" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="81" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="54" t="s">
+      <c r="D26" s="60" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1">
+      <c r="A27" s="74"/>
+      <c r="B27" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="54" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="73" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="63"/>
-      <c r="B27" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="D27" s="75" t="s">
+      <c r="C27" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" s="62" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2975,6 +2971,8 @@
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="F12:F15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
@@ -2983,8 +2981,6 @@
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>